<commit_message>
Implemented pdf generator for trainees
</commit_message>
<xml_diff>
--- a/samples/sample_excel_sheet.xlsx
+++ b/samples/sample_excel_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://intimetecvisionsoft-my.sharepoint.com/personal/anuj_j_intimetec_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wordToPdf\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="73" documentId="8_{A7D94E5A-38CD-4BBC-B7D1-E7755D7F2E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6344711-571C-4731-9544-3FF625D4B766}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DC6C372-DE66-43AF-965D-0FAB274774A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6E3B9890-34E2-4B4A-8915-E48360C036C6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6E3B9890-34E2-4B4A-8915-E48360C036C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -651,22 +651,22 @@
   <dimension ref="A1:J101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.08984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="72.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45838</v>
       </c>
@@ -730,7 +730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45874</v>
       </c>
@@ -762,7 +762,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45838</v>
       </c>
@@ -794,7 +794,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45874</v>
       </c>
@@ -826,7 +826,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45838</v>
       </c>
@@ -858,7 +858,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45874</v>
       </c>
@@ -890,7 +890,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45838</v>
       </c>
@@ -922,7 +922,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45874</v>
       </c>
@@ -954,7 +954,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45838</v>
       </c>
@@ -986,7 +986,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45874</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45838</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45874</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45838</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45874</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45838</v>
       </c>
@@ -1178,7 +1178,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45874</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45838</v>
       </c>
@@ -1242,7 +1242,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45874</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45838</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45874</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45838</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45874</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45838</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45874</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45838</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45874</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45838</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45874</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45838</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45874</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45838</v>
       </c>
@@ -1690,7 +1690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45874</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45838</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45874</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45838</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45874</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45838</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45874</v>
       </c>
@@ -1914,7 +1914,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45838</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45874</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45838</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45874</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45838</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45874</v>
       </c>
@@ -2106,7 +2106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45838</v>
       </c>
@@ -2138,7 +2138,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45874</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45838</v>
       </c>
@@ -2202,7 +2202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45874</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45838</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45874</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45838</v>
       </c>
@@ -2330,7 +2330,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45874</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45838</v>
       </c>
@@ -2394,7 +2394,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45874</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45838</v>
       </c>
@@ -2458,7 +2458,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45874</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45838</v>
       </c>
@@ -2522,7 +2522,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45874</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45838</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45874</v>
       </c>
@@ -2618,7 +2618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45838</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45874</v>
       </c>
@@ -2682,7 +2682,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45838</v>
       </c>
@@ -2714,7 +2714,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45874</v>
       </c>
@@ -2746,7 +2746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45838</v>
       </c>
@@ -2778,7 +2778,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45874</v>
       </c>
@@ -2810,7 +2810,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45838</v>
       </c>
@@ -2842,7 +2842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45874</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45838</v>
       </c>
@@ -2906,7 +2906,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45874</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45838</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45874</v>
       </c>
@@ -3002,7 +3002,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45838</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45874</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45838</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45874</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45838</v>
       </c>
@@ -3162,7 +3162,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45874</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45838</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45874</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45838</v>
       </c>
@@ -3290,7 +3290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45874</v>
       </c>
@@ -3322,7 +3322,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45838</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45874</v>
       </c>
@@ -3386,7 +3386,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45838</v>
       </c>
@@ -3418,7 +3418,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45874</v>
       </c>
@@ -3450,7 +3450,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>45838</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>45874</v>
       </c>
@@ -3514,7 +3514,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>45838</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>45874</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>45838</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>45874</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>45838</v>
       </c>
@@ -3674,7 +3674,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>45874</v>
       </c>
@@ -3706,7 +3706,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>45838</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>45874</v>
       </c>
@@ -3770,7 +3770,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>45838</v>
       </c>
@@ -3802,7 +3802,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>45874</v>
       </c>
@@ -3834,7 +3834,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>45838</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>45874</v>
       </c>

</xml_diff>